<commit_message>
Added Generation times in Readme and modified excel file
</commit_message>
<xml_diff>
--- a/graphs-sorts.xlsx
+++ b/graphs-sorts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapti\Desktop\Documents\Scolarite\EiCnam\1ere_annee\algorithmique-et-programmation\TP\tp-python-algo-tri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F66948-8076-4C71-8963-32AED5613602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E07DC1-1BB2-4AF5-AFA0-EBB7B5A5621C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5F0BF129-34DD-49C2-B73B-CA61EFD8D5D8}"/>
   </bookViews>
@@ -36,42 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Entries</t>
   </si>
   <si>
-    <t>0.7310469150543213</t>
-  </si>
-  <si>
-    <t>1.1986496448516846</t>
-  </si>
-  <si>
-    <t>1.6297695636749268</t>
-  </si>
-  <si>
-    <t>2.190520763397217</t>
-  </si>
-  <si>
-    <t>2.74592661857605</t>
-  </si>
-  <si>
-    <t>3.341700553894043</t>
-  </si>
-  <si>
-    <t>3.849144697189331</t>
-  </si>
-  <si>
-    <t>5.432266473770142</t>
-  </si>
-  <si>
-    <t>4.8259007930755615</t>
-  </si>
-  <si>
-    <t>4.3899266719818115</t>
-  </si>
-  <si>
-    <t>Execution times (s)</t>
+    <t>Execution Times (s)</t>
   </si>
 </sst>
 </file>
@@ -142,14 +112,966 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Feuil1!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.73104691505432096</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1986496448516799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6297695636749201</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1905207633972101</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7459266185760498</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.3417005538940399</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.8491446971893302</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.3899266719818097</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.8259007930755597</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.4322664737701398</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3474-4FE2-9F26-319495AC3686}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1735076528"/>
+        <c:axId val="1603781184"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1735076528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1603781184"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1603781184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1735076528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.25"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>982980</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>140962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>140962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F545362-3C4B-14AA-7420-E97090AF45F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7242B67E-C3CD-4A5A-BB7E-AA01784398EF}" name="Tableau2" displayName="Tableau2" ref="A1:B11" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:B11" xr:uid="{7242B67E-C3CD-4A5A-BB7E-AA01784398EF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D0D0DC6-8CA9-4717-990A-0B184C90866C}" name="Tableau1" displayName="Tableau1" ref="B1:C11" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="B1:C11" xr:uid="{7D0D0DC6-8CA9-4717-990A-0B184C90866C}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{BEE2935C-46B6-4610-8FBA-1373340AD190}" name="Entries" dataDxfId="3">
-      <calculatedColumnFormula>A1+1000000</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{702C1C2F-4FF5-4541-9794-D2267B820726}" name="Entries" dataDxfId="1">
+      <calculatedColumnFormula>B1+1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{8242D32D-487E-4A9D-B6B4-A3B173371AD9}" name="Execution times (s)" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{28487BF3-414E-4B88-9A5D-433A3D7B0304}" name="Execution Times (s)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -452,120 +1374,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C73928-2905-441D-B8B2-2E458610416F}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="B1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.77734375" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="5" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="1">
         <v>1000000</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
+      <c r="C2" s="1">
+        <v>0.73104691505432096</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <f>A2+1000000</f>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="1">
+        <f>B2+1000000</f>
         <v>2000000</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
+      <c r="C3" s="1">
+        <v>1.1986496448516799</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <f>A3+1000000</f>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="1">
+        <f t="shared" ref="B4:B11" si="0">B3+1000000</f>
         <v>3000000</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
+      <c r="C4" s="1">
+        <v>1.6297695636749201</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <f>A4+1000000</f>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
         <v>4000000</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
+      <c r="C5" s="1">
+        <v>2.1905207633972101</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <f>A5+1000000</f>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
         <v>5000000</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
+      <c r="C6" s="1">
+        <v>2.7459266185760498</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <f>A6+1000000</f>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
         <v>6000000</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
+      <c r="C7" s="1">
+        <v>3.3417005538940399</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <f>A7+1000000</f>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
         <v>7000000</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
+      <c r="C8" s="1">
+        <v>3.8491446971893302</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <f>A8+1000000</f>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
         <v>8000000</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
+      <c r="C9" s="1">
+        <v>4.3899266719818097</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <f>A9+1000000</f>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
         <v>9000000</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
+      <c r="C10" s="1">
+        <v>4.8259007930755597</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <f>A10+1000000</f>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
+      <c r="C11" s="1">
+        <v>5.4322664737701398</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>